<commit_message>
isolated Customer data into a seperate tab
</commit_message>
<xml_diff>
--- a/ExcelTemplates/StundenzettelTemplate.xlsx
+++ b/ExcelTemplates/StundenzettelTemplate.xlsx
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -161,6 +161,20 @@
     <font>
       <b/>
       <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -496,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="141">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -643,6 +657,99 @@
     <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="31" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="2" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="14" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="11" fillId="3" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="11" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="17" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="18" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="16" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="11" fillId="4" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="11" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="17" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="18" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="16" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="19" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="21" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="22" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="23" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="25" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="25" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="26" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="27" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="28" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="30" fillId="6" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="11" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="0" fontId="10" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="22" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="25" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="22" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="4" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -2332,62 +2439,62 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C6:G7"/>
-    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A21:I22"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A25:O25"/>
+    <mergeCell ref="A26:O26"/>
+    <mergeCell ref="A27:O27"/>
+    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="A30:O30"/>
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="A32:O32"/>
     <mergeCell ref="A33:O33"/>
     <mergeCell ref="A34:O34"/>
-    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="A35:O35"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:G7"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
     <mergeCell ref="J36:O38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A26:O26"/>
-    <mergeCell ref="A35:O35"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="A21:I22"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="A24:O24"/>
-    <mergeCell ref="A25:O25"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="A27:O27"/>
-    <mergeCell ref="A28:O28"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -3819,17 +3926,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
     <mergeCell ref="A21:I22"/>
     <mergeCell ref="A23:O23"/>
     <mergeCell ref="A24:O24"/>
@@ -3837,9 +3933,6 @@
     <mergeCell ref="A26:O26"/>
     <mergeCell ref="A27:O27"/>
     <mergeCell ref="A28:O28"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="J36:O38"/>
-    <mergeCell ref="C38:D38"/>
     <mergeCell ref="A29:O29"/>
     <mergeCell ref="A30:O30"/>
     <mergeCell ref="A31:O31"/>
@@ -3847,8 +3940,6 @@
     <mergeCell ref="A33:O33"/>
     <mergeCell ref="A34:O34"/>
     <mergeCell ref="A35:O35"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:N7"/>
@@ -3858,23 +3949,39 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:G7"/>
     <mergeCell ref="H6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J36:O38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -5306,62 +5413,62 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:G7"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
     <mergeCell ref="A21:I22"/>
     <mergeCell ref="A23:O23"/>
     <mergeCell ref="A24:O24"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="A25:O25"/>
+    <mergeCell ref="A26:O26"/>
+    <mergeCell ref="A27:O27"/>
+    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="A29:O29"/>
     <mergeCell ref="A30:O30"/>
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="A32:O32"/>
     <mergeCell ref="A33:O33"/>
     <mergeCell ref="A34:O34"/>
     <mergeCell ref="A35:O35"/>
-    <mergeCell ref="A25:O25"/>
-    <mergeCell ref="A26:O26"/>
-    <mergeCell ref="A27:O27"/>
-    <mergeCell ref="A28:O28"/>
-    <mergeCell ref="J36:O38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:G7"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C15:G15"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="J36:O38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -6793,62 +6900,62 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A21:I22"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A25:O25"/>
+    <mergeCell ref="A26:O26"/>
     <mergeCell ref="A27:O27"/>
     <mergeCell ref="A28:O28"/>
-    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A29:O29"/>
     <mergeCell ref="A30:O30"/>
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="A32:O32"/>
     <mergeCell ref="A33:O33"/>
     <mergeCell ref="A34:O34"/>
     <mergeCell ref="A35:O35"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:G7"/>
     <mergeCell ref="H6:I7"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
     <mergeCell ref="H12:I12"/>
+    <mergeCell ref="C13:G13"/>
     <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:I20"/>
-    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
     <mergeCell ref="J36:O38"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="A21:I22"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="A25:O25"/>
-    <mergeCell ref="A26:O26"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -6956,180 +7063,180 @@
       <c r="O7" s="14"/>
     </row>
     <row r="8">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
+      <c r="H8" s="84"/>
       <c r="I8" s="23"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
     </row>
     <row r="9">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="90"/>
       <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
+      <c r="H9" s="91"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="95"/>
+      <c r="N9" s="95"/>
+      <c r="O9" s="95"/>
     </row>
     <row r="10">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
+      <c r="A10" s="96"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
+      <c r="H10" s="98"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="102"/>
     </row>
     <row r="11">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="90"/>
       <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="H11" s="91"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="95"/>
+      <c r="N11" s="95"/>
+      <c r="O11" s="95"/>
     </row>
     <row r="12">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
+      <c r="A12" s="96"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="97"/>
       <c r="G12" s="40"/>
-      <c r="H12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
+      <c r="H12" s="98"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="102"/>
     </row>
     <row r="13">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="90"/>
       <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
+      <c r="H13" s="91"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="95"/>
+      <c r="N13" s="95"/>
+      <c r="O13" s="95"/>
     </row>
     <row r="14">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
+      <c r="A14" s="96"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="97"/>
       <c r="G14" s="40"/>
-      <c r="H14" s="41"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
+      <c r="H14" s="98"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
+      <c r="A15" s="89"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="90"/>
       <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
+      <c r="H15" s="91"/>
+      <c r="J15" s="92"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="95"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="95"/>
     </row>
     <row r="16">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="A16" s="96"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
       <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
+      <c r="H16" s="98"/>
+      <c r="J16" s="99"/>
+      <c r="K16" s="100"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="102"/>
     </row>
     <row r="17">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
+      <c r="A17" s="89"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="90"/>
       <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
+      <c r="H17" s="91"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="95"/>
+      <c r="N17" s="95"/>
+      <c r="O17" s="95"/>
     </row>
     <row r="18">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
+      <c r="A18" s="96"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
       <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
+      <c r="H18" s="98"/>
+      <c r="J18" s="99"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="101"/>
+      <c r="M18" s="102"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="102"/>
     </row>
     <row r="19">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="90"/>
       <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
+      <c r="H19" s="91"/>
+      <c r="J19" s="92"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="94"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="95"/>
+      <c r="O19" s="95"/>
     </row>
     <row r="20">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
+      <c r="A20" s="96"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
       <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
+      <c r="H20" s="98"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="101"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="102"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="103" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="47"/>
@@ -7140,20 +7247,20 @@
       <c r="G21" s="47"/>
       <c r="H21" s="47"/>
       <c r="I21" s="47"/>
-      <c r="J21" s="48" t="s">
+      <c r="J21" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="49" t="s">
+      <c r="K21" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="50" t="s">
+      <c r="L21" s="106" t="s">
         <v>16</v>
       </c>
       <c r="M21" s="51"/>
-      <c r="N21" s="52" t="s">
+      <c r="N21" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="O21" s="53" t="s">
+      <c r="O21" s="108" t="s">
         <v>18</v>
       </c>
     </row>
@@ -7167,15 +7274,15 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="56"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="110"/>
+      <c r="L22" s="111"/>
       <c r="M22" s="57"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
+      <c r="N22" s="112"/>
+      <c r="O22" s="112"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="59"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
@@ -7195,54 +7302,54 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="63"/>
+      <c r="A24" s="114"/>
       <c r="O24" s="64"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="65"/>
+      <c r="A25" s="115"/>
       <c r="O25" s="64"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="63"/>
+      <c r="A26" s="114"/>
       <c r="O26" s="64"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="65"/>
+      <c r="A27" s="115"/>
       <c r="O27" s="64"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="63"/>
+      <c r="A28" s="114"/>
       <c r="O28" s="64"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="65"/>
+      <c r="A29" s="115"/>
       <c r="O29" s="64"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="63"/>
+      <c r="A30" s="114"/>
       <c r="O30" s="64"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="65"/>
+      <c r="A31" s="115"/>
       <c r="O31" s="64"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="63"/>
+      <c r="A32" s="114"/>
       <c r="O32" s="64"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="65"/>
+      <c r="A33" s="115"/>
       <c r="O33" s="64"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="63"/>
+      <c r="A34" s="114"/>
       <c r="O34" s="64"/>
       <c r="Q34" s="62" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="66"/>
+      <c r="A35" s="116"/>
       <c r="B35" s="67"/>
       <c r="C35" s="67"/>
       <c r="D35" s="67"/>
@@ -7259,19 +7366,20 @@
       <c r="O35" s="69"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="72" t="s">
+      <c r="B36" s="118"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="119"/>
+      <c r="F36" s="119"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="119"/>
+      <c r="I36" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="73"/>
+      <c r="J36" s="122"/>
       <c r="K36" s="60"/>
       <c r="L36" s="60"/>
       <c r="M36" s="60"/>
@@ -7279,32 +7387,33 @@
       <c r="O36" s="61"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="74"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="72" t="s">
+      <c r="A37" s="123"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="119"/>
+      <c r="E37" s="119"/>
+      <c r="F37" s="119"/>
+      <c r="G37" s="120"/>
+      <c r="H37" s="119"/>
+      <c r="I37" s="121" t="s">
         <v>22</v>
       </c>
       <c r="O37" s="64"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="77" t="s">
+      <c r="B38" s="125"/>
+      <c r="C38" s="126" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="78"/>
-      <c r="E38" s="79"/>
+      <c r="E38" s="127"/>
       <c r="F38" s="80"/>
       <c r="G38" s="80"/>
       <c r="H38" s="78"/>
-      <c r="I38" s="81"/>
+      <c r="I38" s="128"/>
       <c r="J38" s="68"/>
       <c r="K38" s="68"/>
       <c r="L38" s="68"/>
@@ -8280,62 +8389,62 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A21:I22"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A25:O25"/>
+    <mergeCell ref="A26:O26"/>
+    <mergeCell ref="A27:O27"/>
+    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="A31:O31"/>
+    <mergeCell ref="A32:O32"/>
+    <mergeCell ref="A33:O33"/>
     <mergeCell ref="A34:O34"/>
     <mergeCell ref="A35:O35"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="J36:O38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:G7"/>
     <mergeCell ref="H6:I7"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
     <mergeCell ref="H12:I12"/>
+    <mergeCell ref="C13:G13"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C14:G14"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="L22:M22"/>
-    <mergeCell ref="A25:O25"/>
-    <mergeCell ref="A26:O26"/>
-    <mergeCell ref="A27:O27"/>
-    <mergeCell ref="A28:O28"/>
-    <mergeCell ref="A30:O30"/>
-    <mergeCell ref="A31:O31"/>
-    <mergeCell ref="A32:O32"/>
-    <mergeCell ref="A33:O33"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="A21:I22"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A24:O24"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J36:O38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -8377,60 +8486,60 @@
       <c r="G1" s="61"/>
     </row>
     <row r="2">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83"/>
+      <c r="A2" s="129"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="130"/>
       <c r="F2" s="68"/>
       <c r="G2" s="69"/>
     </row>
     <row r="3">
-      <c r="A3" s="84"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87"/>
+      <c r="A3" s="131"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="134"/>
       <c r="F3" s="60"/>
       <c r="G3" s="61"/>
     </row>
     <row r="4">
-      <c r="A4" s="88"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="89"/>
+      <c r="A4" s="135"/>
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="136"/>
       <c r="G4" s="64"/>
     </row>
     <row r="5">
-      <c r="A5" s="86"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="90"/>
+      <c r="A5" s="133"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="137"/>
       <c r="G5" s="64"/>
     </row>
     <row r="6">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="89"/>
+      <c r="A6" s="135"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="136"/>
       <c r="G6" s="64"/>
     </row>
     <row r="7">
-      <c r="A7" s="91"/>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91"/>
-      <c r="E7" s="92"/>
+      <c r="A7" s="138"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="139"/>
       <c r="F7" s="68"/>
       <c r="G7" s="69"/>
     </row>
     <row r="8">
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
introduced and fixed multiple app breaking bugs, made some changes
</commit_message>
<xml_diff>
--- a/ExcelTemplates/StundenzettelTemplate.xlsx
+++ b/ExcelTemplates/StundenzettelTemplate.xlsx
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -135,11 +135,6 @@
       <name val="Calibri"/>
     </font>
     <font/>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -194,14 +189,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -510,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="125">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -526,11 +521,8 @@
     <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -540,36 +532,45 @@
     <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="6" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="3" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="11" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="18" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="16" fillId="4" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="4" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="15" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
@@ -579,24 +580,10 @@
     </xf>
     <xf borderId="16" fillId="3" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="15" fillId="3" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="11" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="18" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="16" fillId="4" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="19" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="20" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="20" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="21" fillId="5" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,10 +593,7 @@
     <xf borderId="23" fillId="5" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="24" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf borderId="24" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="25" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,30 +606,23 @@
     <xf borderId="28" fillId="6" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="29" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="29" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="30" fillId="6" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="9" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -653,23 +630,35 @@
     <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="31" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="14" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="3" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="14" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="6" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="11" fillId="4" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="11" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="17" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="18" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="16" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="15" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
@@ -683,19 +672,6 @@
     </xf>
     <xf borderId="16" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="15" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="11" fillId="4" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="11" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="17" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="18" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="16" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="19" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -711,36 +687,33 @@
     <xf borderId="25" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="25" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="26" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="27" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="28" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="30" fillId="6" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="11" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="11" fillId="0" fontId="10" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="0" fontId="10" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="0" fontId="9" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="22" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -750,33 +723,31 @@
     </xf>
     <xf borderId="22" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="7" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="15" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="15" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="15" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="8" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="7" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -786,36 +757,173 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4124325" cy="904875"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.jpg" title="Bild"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4124325" cy="904875"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.jpg" title="Bild"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4124325" cy="904875"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.jpg" title="Bild"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4124325" cy="904875"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.jpg" title="Bild"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4124325" cy="904875"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.jpg" title="Bild"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1073,412 +1181,412 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
     </row>
     <row r="10">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="37"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
     </row>
     <row r="11">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
     </row>
     <row r="12">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="37"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
     </row>
     <row r="13">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
     </row>
     <row r="14">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="37"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
     </row>
     <row r="15">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
     </row>
     <row r="16">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="37"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
     </row>
     <row r="17">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
     </row>
     <row r="18">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="37"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
     </row>
     <row r="19">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
     </row>
     <row r="20">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="37"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="49" t="s">
+      <c r="K21" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="50" t="s">
+      <c r="L21" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="51"/>
-      <c r="N21" s="52" t="s">
+      <c r="M21" s="47"/>
+      <c r="N21" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="O21" s="53" t="s">
+      <c r="O21" s="48" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="59"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="61"/>
-      <c r="Q23" s="62" t="s">
+      <c r="A23" s="54"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="Q23" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="63"/>
-      <c r="O24" s="64"/>
+      <c r="A24" s="55"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="65"/>
-      <c r="O25" s="64"/>
+      <c r="A25" s="56"/>
+      <c r="O25" s="29"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="63"/>
-      <c r="O26" s="64"/>
+      <c r="A26" s="55"/>
+      <c r="O26" s="29"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="65"/>
-      <c r="O27" s="64"/>
+      <c r="A27" s="56"/>
+      <c r="O27" s="29"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="63"/>
-      <c r="O28" s="64"/>
+      <c r="A28" s="55"/>
+      <c r="O28" s="29"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="65"/>
-      <c r="O29" s="64"/>
+      <c r="A29" s="56"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="63"/>
-      <c r="O30" s="64"/>
+      <c r="A30" s="55"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="65"/>
-      <c r="O31" s="64"/>
+      <c r="A31" s="56"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="63"/>
-      <c r="O32" s="64"/>
+      <c r="A32" s="55"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="65"/>
-      <c r="O33" s="64"/>
+      <c r="A33" s="56"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="63"/>
-      <c r="O34" s="64"/>
-      <c r="Q34" s="62" t="s">
+      <c r="A34" s="55"/>
+      <c r="O34" s="29"/>
+      <c r="Q34" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="66"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="67"/>
-      <c r="N35" s="68"/>
-      <c r="O35" s="69"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="72" t="s">
+      <c r="I36" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="73"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="74"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="72" t="s">
+      <c r="I37" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="64"/>
+      <c r="O37" s="29"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="77" t="s">
+      <c r="B38" s="64"/>
+      <c r="C38" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="78"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="81"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="69"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="13"/>
+      <c r="A39" s="12"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="62"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -2560,412 +2668,412 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
     </row>
     <row r="10">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="37"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
     </row>
     <row r="11">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
     </row>
     <row r="12">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="37"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
     </row>
     <row r="13">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
     </row>
     <row r="14">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="37"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
     </row>
     <row r="15">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
     </row>
     <row r="16">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="37"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
     </row>
     <row r="17">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
     </row>
     <row r="18">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="37"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
     </row>
     <row r="19">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
     </row>
     <row r="20">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="37"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="49" t="s">
+      <c r="K21" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="50" t="s">
+      <c r="L21" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="51"/>
-      <c r="N21" s="52" t="s">
+      <c r="M21" s="47"/>
+      <c r="N21" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="O21" s="53" t="s">
+      <c r="O21" s="48" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="59"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="61"/>
-      <c r="Q23" s="62" t="s">
+      <c r="A23" s="54"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="Q23" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="63"/>
-      <c r="O24" s="64"/>
+      <c r="A24" s="55"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="65"/>
-      <c r="O25" s="64"/>
+      <c r="A25" s="56"/>
+      <c r="O25" s="29"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="63"/>
-      <c r="O26" s="64"/>
+      <c r="A26" s="55"/>
+      <c r="O26" s="29"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="65"/>
-      <c r="O27" s="64"/>
+      <c r="A27" s="56"/>
+      <c r="O27" s="29"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="63"/>
-      <c r="O28" s="64"/>
+      <c r="A28" s="55"/>
+      <c r="O28" s="29"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="65"/>
-      <c r="O29" s="64"/>
+      <c r="A29" s="56"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="63"/>
-      <c r="O30" s="64"/>
+      <c r="A30" s="55"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="65"/>
-      <c r="O31" s="64"/>
+      <c r="A31" s="56"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="63"/>
-      <c r="O32" s="64"/>
+      <c r="A32" s="55"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="65"/>
-      <c r="O33" s="64"/>
+      <c r="A33" s="56"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="63"/>
-      <c r="O34" s="64"/>
-      <c r="Q34" s="62" t="s">
+      <c r="A34" s="55"/>
+      <c r="O34" s="29"/>
+      <c r="Q34" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="66"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="67"/>
-      <c r="N35" s="68"/>
-      <c r="O35" s="69"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="72" t="s">
+      <c r="I36" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="73"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="74"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="72" t="s">
+      <c r="I37" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="64"/>
+      <c r="O37" s="29"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="77" t="s">
+      <c r="B38" s="64"/>
+      <c r="C38" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="78"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="81"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="69"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="13"/>
+      <c r="A39" s="12"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="62"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -4047,412 +4155,412 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
     </row>
     <row r="10">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="37"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
     </row>
     <row r="11">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
     </row>
     <row r="12">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="37"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
     </row>
     <row r="13">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
     </row>
     <row r="14">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="37"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
     </row>
     <row r="15">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
     </row>
     <row r="16">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="37"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
     </row>
     <row r="17">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
     </row>
     <row r="18">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="37"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
     </row>
     <row r="19">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
     </row>
     <row r="20">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="37"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="49" t="s">
+      <c r="K21" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="50" t="s">
+      <c r="L21" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="51"/>
-      <c r="N21" s="52" t="s">
+      <c r="M21" s="47"/>
+      <c r="N21" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="O21" s="53" t="s">
+      <c r="O21" s="48" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="59"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="61"/>
-      <c r="Q23" s="62" t="s">
+      <c r="A23" s="54"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="Q23" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="63"/>
-      <c r="O24" s="64"/>
+      <c r="A24" s="55"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="65"/>
-      <c r="O25" s="64"/>
+      <c r="A25" s="56"/>
+      <c r="O25" s="29"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="63"/>
-      <c r="O26" s="64"/>
+      <c r="A26" s="55"/>
+      <c r="O26" s="29"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="65"/>
-      <c r="O27" s="64"/>
+      <c r="A27" s="56"/>
+      <c r="O27" s="29"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="63"/>
-      <c r="O28" s="64"/>
+      <c r="A28" s="55"/>
+      <c r="O28" s="29"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="65"/>
-      <c r="O29" s="64"/>
+      <c r="A29" s="56"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="63"/>
-      <c r="O30" s="64"/>
+      <c r="A30" s="55"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="65"/>
-      <c r="O31" s="64"/>
+      <c r="A31" s="56"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="63"/>
-      <c r="O32" s="64"/>
+      <c r="A32" s="55"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="65"/>
-      <c r="O33" s="64"/>
+      <c r="A33" s="56"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="63"/>
-      <c r="O34" s="64"/>
-      <c r="Q34" s="62" t="s">
+      <c r="A34" s="55"/>
+      <c r="O34" s="29"/>
+      <c r="Q34" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="66"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="67"/>
-      <c r="N35" s="68"/>
-      <c r="O35" s="69"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="72" t="s">
+      <c r="I36" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="73"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="74"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="72" t="s">
+      <c r="I37" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="64"/>
+      <c r="O37" s="29"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="77" t="s">
+      <c r="B38" s="64"/>
+      <c r="C38" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="78"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="81"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="69"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="13"/>
+      <c r="A39" s="12"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="62"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -5534,412 +5642,412 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
     </row>
     <row r="10">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="37"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
     </row>
     <row r="11">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
     </row>
     <row r="12">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="37"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
     </row>
     <row r="13">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
     </row>
     <row r="14">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="37"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
     </row>
     <row r="15">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
     </row>
     <row r="16">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="37"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
     </row>
     <row r="17">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
     </row>
     <row r="18">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="37"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
     </row>
     <row r="19">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
     </row>
     <row r="20">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="37"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="48" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="49" t="s">
+      <c r="K21" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="50" t="s">
+      <c r="L21" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="51"/>
-      <c r="N21" s="52" t="s">
+      <c r="M21" s="47"/>
+      <c r="N21" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="O21" s="53" t="s">
+      <c r="O21" s="48" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="59"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="61"/>
-      <c r="Q23" s="62" t="s">
+      <c r="A23" s="54"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="Q23" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="63"/>
-      <c r="O24" s="64"/>
+      <c r="A24" s="55"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="65"/>
-      <c r="O25" s="64"/>
+      <c r="A25" s="56"/>
+      <c r="O25" s="29"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="63"/>
-      <c r="O26" s="64"/>
+      <c r="A26" s="55"/>
+      <c r="O26" s="29"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="65"/>
-      <c r="O27" s="64"/>
+      <c r="A27" s="56"/>
+      <c r="O27" s="29"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="63"/>
-      <c r="O28" s="64"/>
+      <c r="A28" s="55"/>
+      <c r="O28" s="29"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="65"/>
-      <c r="O29" s="64"/>
+      <c r="A29" s="56"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="63"/>
-      <c r="O30" s="64"/>
+      <c r="A30" s="55"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="65"/>
-      <c r="O31" s="64"/>
+      <c r="A31" s="56"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="63"/>
-      <c r="O32" s="64"/>
+      <c r="A32" s="55"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="65"/>
-      <c r="O33" s="64"/>
+      <c r="A33" s="56"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="63"/>
-      <c r="O34" s="64"/>
-      <c r="Q34" s="62" t="s">
+      <c r="A34" s="55"/>
+      <c r="O34" s="29"/>
+      <c r="Q34" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="66"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="67"/>
-      <c r="N35" s="68"/>
-      <c r="O35" s="69"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="72" t="s">
+      <c r="I36" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="73"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="74"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="72" t="s">
+      <c r="I37" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="64"/>
+      <c r="O37" s="29"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="77" t="s">
+      <c r="B38" s="64"/>
+      <c r="C38" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="78"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="81"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="69"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="13"/>
+      <c r="A39" s="12"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="62"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -7021,414 +7129,414 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="82"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
     </row>
     <row r="9">
-      <c r="A9" s="89"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="90"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="91"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="95"/>
-      <c r="N9" s="95"/>
-      <c r="O9" s="95"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="77"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="78"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
     </row>
     <row r="10">
-      <c r="A10" s="96"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="97"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="98"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="100"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="102"/>
-      <c r="N10" s="102"/>
-      <c r="O10" s="102"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="85"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
     </row>
     <row r="11">
-      <c r="A11" s="89"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="90"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="91"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="95"/>
-      <c r="N11" s="95"/>
-      <c r="O11" s="95"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="77"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="78"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
     </row>
     <row r="12">
-      <c r="A12" s="96"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="97"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="98"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="100"/>
-      <c r="L12" s="101"/>
-      <c r="M12" s="102"/>
-      <c r="N12" s="102"/>
-      <c r="O12" s="102"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="84"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="85"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
     </row>
     <row r="13">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="90"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="91"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="95"/>
-      <c r="N13" s="95"/>
-      <c r="O13" s="95"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="77"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="78"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
     </row>
     <row r="14">
-      <c r="A14" s="96"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="97"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="98"/>
-      <c r="J14" s="99"/>
-      <c r="K14" s="100"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="102"/>
-      <c r="N14" s="102"/>
-      <c r="O14" s="102"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="84"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="85"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
     </row>
     <row r="15">
-      <c r="A15" s="89"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="90"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="91"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="95"/>
-      <c r="N15" s="95"/>
-      <c r="O15" s="95"/>
+      <c r="A15" s="76"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="77"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="78"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
     </row>
     <row r="16">
-      <c r="A16" s="96"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="97"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="98"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="100"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="84"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="85"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="89"/>
     </row>
     <row r="17">
-      <c r="A17" s="89"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="90"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="91"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="95"/>
-      <c r="N17" s="95"/>
-      <c r="O17" s="95"/>
+      <c r="A17" s="76"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="77"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="78"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
     </row>
     <row r="18">
-      <c r="A18" s="96"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="97"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="98"/>
-      <c r="J18" s="99"/>
-      <c r="K18" s="100"/>
-      <c r="L18" s="101"/>
-      <c r="M18" s="102"/>
-      <c r="N18" s="102"/>
-      <c r="O18" s="102"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="84"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="85"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="89"/>
     </row>
     <row r="19">
-      <c r="A19" s="89"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="91"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="93"/>
-      <c r="L19" s="94"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="95"/>
-      <c r="O19" s="95"/>
+      <c r="A19" s="76"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="77"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="78"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
     </row>
     <row r="20">
-      <c r="A20" s="96"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="97"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="98"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="100"/>
-      <c r="L20" s="101"/>
-      <c r="M20" s="102"/>
-      <c r="N20" s="102"/>
-      <c r="O20" s="102"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="84"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="85"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="89"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="103" t="s">
+      <c r="A21" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="104" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="105" t="s">
+      <c r="K21" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="106" t="s">
+      <c r="L21" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="51"/>
-      <c r="N21" s="107" t="s">
+      <c r="M21" s="47"/>
+      <c r="N21" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="O21" s="108" t="s">
+      <c r="O21" s="94" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="109"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="111"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="112"/>
-      <c r="O22" s="112"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="95"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="98"/>
+      <c r="O22" s="98"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="113"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="61"/>
-      <c r="Q23" s="62" t="s">
+      <c r="A23" s="99"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="Q23" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="114"/>
-      <c r="O24" s="64"/>
+      <c r="A24" s="100"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="115"/>
-      <c r="O25" s="64"/>
+      <c r="A25" s="101"/>
+      <c r="O25" s="29"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="114"/>
-      <c r="O26" s="64"/>
+      <c r="A26" s="100"/>
+      <c r="O26" s="29"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="115"/>
-      <c r="O27" s="64"/>
+      <c r="A27" s="101"/>
+      <c r="O27" s="29"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="114"/>
-      <c r="O28" s="64"/>
+      <c r="A28" s="100"/>
+      <c r="O28" s="29"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="115"/>
-      <c r="O29" s="64"/>
+      <c r="A29" s="101"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="114"/>
-      <c r="O30" s="64"/>
+      <c r="A30" s="100"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="115"/>
-      <c r="O31" s="64"/>
+      <c r="A31" s="101"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="114"/>
-      <c r="O32" s="64"/>
+      <c r="A32" s="100"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="115"/>
-      <c r="O33" s="64"/>
+      <c r="A33" s="101"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="114"/>
-      <c r="O34" s="64"/>
-      <c r="Q34" s="62" t="s">
+      <c r="A34" s="100"/>
+      <c r="O34" s="29"/>
+      <c r="Q34" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="116"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="67"/>
-      <c r="N35" s="68"/>
-      <c r="O35" s="69"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="117" t="s">
+      <c r="A36" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="118"/>
-      <c r="C36" s="118"/>
-      <c r="D36" s="118"/>
-      <c r="E36" s="119"/>
-      <c r="F36" s="119"/>
-      <c r="G36" s="120"/>
-      <c r="H36" s="119"/>
-      <c r="I36" s="121" t="s">
+      <c r="B36" s="104"/>
+      <c r="C36" s="104"/>
+      <c r="D36" s="104"/>
+      <c r="E36" s="105"/>
+      <c r="F36" s="105"/>
+      <c r="G36" s="106"/>
+      <c r="H36" s="105"/>
+      <c r="I36" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="J36" s="122"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="61"/>
+      <c r="J36" s="108"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="123"/>
-      <c r="B37" s="119"/>
-      <c r="C37" s="119"/>
-      <c r="D37" s="119"/>
-      <c r="E37" s="119"/>
-      <c r="F37" s="119"/>
-      <c r="G37" s="120"/>
-      <c r="H37" s="119"/>
-      <c r="I37" s="121" t="s">
+      <c r="A37" s="109"/>
+      <c r="B37" s="105"/>
+      <c r="C37" s="105"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="105"/>
+      <c r="F37" s="105"/>
+      <c r="G37" s="106"/>
+      <c r="H37" s="105"/>
+      <c r="I37" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="64"/>
+      <c r="O37" s="29"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="124" t="s">
+      <c r="A38" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="125"/>
-      <c r="C38" s="126" t="s">
+      <c r="B38" s="111"/>
+      <c r="C38" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="78"/>
-      <c r="E38" s="127"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="128"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="69"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="114"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="13"/>
+      <c r="A39" s="12"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="62"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -8482,64 +8590,64 @@
       <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="61"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2">
-      <c r="A2" s="129"/>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="69"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3">
-      <c r="A3" s="131"/>
-      <c r="B3" s="131"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="133"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="A3" s="115"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4">
-      <c r="A4" s="135"/>
-      <c r="B4" s="135"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="136"/>
-      <c r="G4" s="64"/>
+      <c r="A4" s="119"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="120"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5">
-      <c r="A5" s="133"/>
-      <c r="B5" s="133"/>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="137"/>
-      <c r="G5" s="64"/>
+      <c r="A5" s="117"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="121"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6">
-      <c r="A6" s="135"/>
-      <c r="B6" s="135"/>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="136"/>
-      <c r="G6" s="64"/>
+      <c r="A6" s="119"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="120"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7">
-      <c r="A7" s="138"/>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8">
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
+      <c r="B8" s="124"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="124"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
isolated car load time and privately driven km
</commit_message>
<xml_diff>
--- a/ExcelTemplates/StundenzettelTemplate.xlsx
+++ b/ExcelTemplates/StundenzettelTemplate.xlsx
@@ -5,7 +5,7 @@
   <sheets>
     <sheet state="visible" name="Montag" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Dienstag" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Mittwochh" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Mittwoch" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Donnerstag" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Freitag" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="Wertezusammenfassung" sheetId="6" r:id="rId9"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="32">
   <si>
     <t>Rapportzettel :</t>
   </si>
@@ -45,6 +45,10 @@
     <t>Pause</t>
   </si>
   <si>
+    <t>Lade
+Zeit</t>
+  </si>
+  <si>
     <t>Km
 Beginn</t>
   </si>
@@ -53,28 +57,20 @@
 Ende</t>
   </si>
   <si>
-    <t>Dienstfahrt</t>
-  </si>
-  <si>
-    <t>Privatfahrt</t>
+    <t>Km
+Privatfahrt</t>
   </si>
   <si>
     <t>Arbeitsbeschreibung</t>
   </si>
   <si>
-    <t>Arbeitszeit</t>
+    <t>Ges.</t>
   </si>
   <si>
-    <t xml:space="preserve">Pause </t>
+    <t>Ges</t>
   </si>
   <si>
-    <t>Gesamt km</t>
-  </si>
-  <si>
-    <t>Ge. Km</t>
-  </si>
-  <si>
-    <t>Ge.Km</t>
+    <t>Ges. km</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -98,14 +94,35 @@
     <t>Datum</t>
   </si>
   <si>
+    <t>Arbeitszeit</t>
+  </si>
+  <si>
+    <t>Laden</t>
+  </si>
+  <si>
+    <t>Gesamt km</t>
+  </si>
+  <si>
+    <t>Privat km</t>
+  </si>
+  <si>
     <t>Fahrzeug</t>
+  </si>
+  <si>
+    <t>Ges. Arbeitszeit</t>
+  </si>
+  <si>
+    <t>Ges. Pause</t>
+  </si>
+  <si>
+    <t>Ges. Laden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -154,22 +171,13 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -189,14 +197,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -212,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="28">
     <border/>
     <border>
       <left style="thin">
@@ -250,17 +258,6 @@
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -311,17 +308,6 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
@@ -350,14 +336,6 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
         <color rgb="FF000000"/>
       </right>
     </border>
@@ -483,17 +461,6 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -505,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="67">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -515,249 +482,155 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="4" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="12" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="18" fillId="4" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="3" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="16" fillId="4" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="15" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="18" fillId="3" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="16" fillId="3" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="3" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="19" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="5" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="4" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="22" fillId="5" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="23" fillId="5" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="26" fillId="6" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="27" fillId="6" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="28" fillId="6" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="29" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="30" fillId="6" fontId="2" numFmtId="1" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="31" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="14" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="15" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="4" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="11" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="17" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="16" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="18" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="19" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="20" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="21" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="22" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="23" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="18" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="24" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="16" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="25" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="6" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="11" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="17" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+    <xf borderId="26" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="18" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="16" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="3" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="19" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="21" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="22" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="23" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="25" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="26" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="27" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="28" fillId="6" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="30" fillId="6" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="10" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="10" fillId="0" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="0" fontId="9" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="13" fillId="0" fontId="10" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="22" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="25" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="22" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="19" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="19" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="22" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="27" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="27" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="15" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="15" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="11" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="7" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="6" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1188,261 +1061,261 @@
       <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="13"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="22"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="37"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
     </row>
     <row r="11">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="30"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
     </row>
     <row r="13">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
     </row>
     <row r="14">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="37"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
     </row>
     <row r="16">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="37"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
     </row>
     <row r="17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
     </row>
     <row r="18">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="37"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
     </row>
     <row r="19">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
     </row>
     <row r="20">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="37"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="44" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="45" t="s">
+      <c r="K21" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="O21" s="48" t="s">
-        <v>18</v>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="40"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="54"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1457,88 +1330,89 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="8"/>
-      <c r="Q23" s="12" t="s">
+      <c r="Q23" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="44"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="45"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="45"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="O28" s="25"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="45"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="44"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="O31" s="25"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="44"/>
+      <c r="O32" s="25"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="45"/>
+      <c r="O33" s="25"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="44"/>
+      <c r="O34" s="25"/>
+      <c r="Q34" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="46"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="15"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="51" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="55"/>
-      <c r="O24" s="29"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="56"/>
-      <c r="O25" s="29"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="55"/>
-      <c r="O26" s="29"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="56"/>
-      <c r="O27" s="29"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="55"/>
-      <c r="O28" s="29"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="56"/>
-      <c r="O29" s="29"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="55"/>
-      <c r="O30" s="29"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="56"/>
-      <c r="O31" s="29"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="55"/>
-      <c r="O32" s="29"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="56"/>
-      <c r="O33" s="29"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="55"/>
-      <c r="O34" s="29"/>
-      <c r="Q34" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="57"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="16"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="61"/>
+      <c r="J36" s="52"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -1546,47 +1420,50 @@
       <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="62"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="60" t="s">
+      <c r="A37" s="53"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="O37" s="25"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="55"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="29"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="16"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="15"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="12"/>
+      <c r="A39" s="11"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="C41" s="59"/>
+    </row>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="12"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -2546,63 +2423,65 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A21:I22"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="A24:O24"/>
-    <mergeCell ref="A25:O25"/>
+  <mergeCells count="58">
     <mergeCell ref="A26:O26"/>
     <mergeCell ref="A27:O27"/>
-    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A21:I22"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="A29:O29"/>
     <mergeCell ref="A30:O30"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A34:O34"/>
+    <mergeCell ref="A35:O35"/>
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="A32:O32"/>
     <mergeCell ref="A33:O33"/>
-    <mergeCell ref="A34:O34"/>
-    <mergeCell ref="A35:O35"/>
+    <mergeCell ref="J36:O38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A25:O25"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:G7"/>
-    <mergeCell ref="H6:I7"/>
     <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J36:O38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -2675,261 +2554,261 @@
       <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="13"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="22"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="37"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
     </row>
     <row r="11">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="30"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
     </row>
     <row r="13">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
     </row>
     <row r="14">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="37"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
     </row>
     <row r="16">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="37"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
     </row>
     <row r="17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
     </row>
     <row r="18">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="37"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
     </row>
     <row r="19">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
     </row>
     <row r="20">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="37"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="44" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="45" t="s">
+      <c r="K21" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="O21" s="48" t="s">
-        <v>18</v>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="40"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="54"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -2944,88 +2823,89 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="8"/>
-      <c r="Q23" s="12" t="s">
+      <c r="Q23" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="44"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="45"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="45"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="O28" s="25"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="45"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="44"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="O31" s="25"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="44"/>
+      <c r="O32" s="25"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="45"/>
+      <c r="O33" s="25"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="44"/>
+      <c r="O34" s="25"/>
+      <c r="Q34" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="46"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="15"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="51" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="55"/>
-      <c r="O24" s="29"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="56"/>
-      <c r="O25" s="29"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="55"/>
-      <c r="O26" s="29"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="56"/>
-      <c r="O27" s="29"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="55"/>
-      <c r="O28" s="29"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="56"/>
-      <c r="O29" s="29"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="55"/>
-      <c r="O30" s="29"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="56"/>
-      <c r="O31" s="29"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="55"/>
-      <c r="O32" s="29"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="56"/>
-      <c r="O33" s="29"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="55"/>
-      <c r="O34" s="29"/>
-      <c r="Q34" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="57"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="16"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="61"/>
+      <c r="J36" s="52"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -3033,47 +2913,50 @@
       <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="62"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="60" t="s">
+      <c r="A37" s="53"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="O37" s="25"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="55"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="29"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="16"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="15"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="12"/>
+      <c r="A39" s="11"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="C41" s="59"/>
+    </row>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="12"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -4033,63 +3916,65 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A21:I22"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="A24:O24"/>
-    <mergeCell ref="A25:O25"/>
-    <mergeCell ref="A26:O26"/>
+  <mergeCells count="58">
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C6:G7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C9:G9"/>
     <mergeCell ref="A27:O27"/>
     <mergeCell ref="A28:O28"/>
+    <mergeCell ref="J36:O38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F38:H38"/>
     <mergeCell ref="A29:O29"/>
     <mergeCell ref="A30:O30"/>
+    <mergeCell ref="A34:O34"/>
+    <mergeCell ref="A35:O35"/>
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="A32:O32"/>
     <mergeCell ref="A33:O33"/>
-    <mergeCell ref="A34:O34"/>
-    <mergeCell ref="A35:O35"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A25:O25"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="A26:O26"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A21:I22"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="C19:G19"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="O6:O7"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:G7"/>
     <mergeCell ref="H6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="H9:I9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J36:O38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -4162,261 +4047,261 @@
       <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="13"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="22"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="37"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
     </row>
     <row r="11">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="30"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
     </row>
     <row r="13">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
     </row>
     <row r="14">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="37"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
     </row>
     <row r="16">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="37"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
     </row>
     <row r="17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
     </row>
     <row r="18">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="37"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
     </row>
     <row r="19">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
     </row>
     <row r="20">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="37"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="44" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="45" t="s">
+      <c r="K21" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="O21" s="48" t="s">
-        <v>18</v>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="40"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="54"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -4431,88 +4316,89 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="8"/>
-      <c r="Q23" s="12" t="s">
+      <c r="Q23" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="44"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="45"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="45"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="O28" s="25"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="45"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="44"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="O31" s="25"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="44"/>
+      <c r="O32" s="25"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="45"/>
+      <c r="O33" s="25"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="44"/>
+      <c r="O34" s="25"/>
+      <c r="Q34" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="46"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="15"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="51" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="55"/>
-      <c r="O24" s="29"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="56"/>
-      <c r="O25" s="29"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="55"/>
-      <c r="O26" s="29"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="56"/>
-      <c r="O27" s="29"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="55"/>
-      <c r="O28" s="29"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="56"/>
-      <c r="O29" s="29"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="55"/>
-      <c r="O30" s="29"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="56"/>
-      <c r="O31" s="29"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="55"/>
-      <c r="O32" s="29"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="56"/>
-      <c r="O33" s="29"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="55"/>
-      <c r="O34" s="29"/>
-      <c r="Q34" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="57"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="16"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="61"/>
+      <c r="J36" s="52"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -4520,47 +4406,50 @@
       <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="62"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="60" t="s">
+      <c r="A37" s="53"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="O37" s="25"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="55"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="29"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="16"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="15"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="12"/>
+      <c r="A39" s="11"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="C41" s="59"/>
+    </row>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="12"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -5520,63 +5409,65 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A21:I22"/>
-    <mergeCell ref="A23:O23"/>
+  <mergeCells count="58">
+    <mergeCell ref="J36:O38"/>
+    <mergeCell ref="A34:O34"/>
+    <mergeCell ref="A35:O35"/>
+    <mergeCell ref="A27:O27"/>
     <mergeCell ref="A24:O24"/>
     <mergeCell ref="A25:O25"/>
     <mergeCell ref="A26:O26"/>
-    <mergeCell ref="A27:O27"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A21:I22"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="A33:O33"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="C6:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C14:G14"/>
     <mergeCell ref="A28:O28"/>
     <mergeCell ref="A29:O29"/>
-    <mergeCell ref="A30:O30"/>
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="A32:O32"/>
-    <mergeCell ref="A33:O33"/>
-    <mergeCell ref="A34:O34"/>
-    <mergeCell ref="A35:O35"/>
+    <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:G7"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="H6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J36:O38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -5649,261 +5540,261 @@
       <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="13"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="22"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="37"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
     </row>
     <row r="11">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="30"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
     </row>
     <row r="13">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
     </row>
     <row r="14">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="37"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
     </row>
     <row r="16">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="37"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
     </row>
     <row r="17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
     </row>
     <row r="18">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="37"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
     </row>
     <row r="19">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
     </row>
     <row r="20">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="37"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="44" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="45" t="s">
+      <c r="K21" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="O21" s="48" t="s">
-        <v>18</v>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="40"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="54"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -5918,88 +5809,89 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="8"/>
-      <c r="Q23" s="12" t="s">
+      <c r="Q23" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="44"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="45"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="45"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="O28" s="25"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="45"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="44"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="O31" s="25"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="44"/>
+      <c r="O32" s="25"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="45"/>
+      <c r="O33" s="25"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="44"/>
+      <c r="O34" s="25"/>
+      <c r="Q34" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="46"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="15"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="51" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="55"/>
-      <c r="O24" s="29"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="56"/>
-      <c r="O25" s="29"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="55"/>
-      <c r="O26" s="29"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="56"/>
-      <c r="O27" s="29"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="55"/>
-      <c r="O28" s="29"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="56"/>
-      <c r="O29" s="29"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="55"/>
-      <c r="O30" s="29"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="56"/>
-      <c r="O31" s="29"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="55"/>
-      <c r="O32" s="29"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="56"/>
-      <c r="O33" s="29"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="55"/>
-      <c r="O34" s="29"/>
-      <c r="Q34" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="57"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="16"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="61"/>
+      <c r="J36" s="52"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -6007,47 +5899,50 @@
       <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="62"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="60" t="s">
+      <c r="A37" s="53"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="O37" s="25"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="55"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="29"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="16"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="15"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="12"/>
+      <c r="A39" s="11"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="C41" s="59"/>
+    </row>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="12"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -7007,63 +6902,65 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="58">
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="C6:G7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A27:O27"/>
+    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C18:G18"/>
     <mergeCell ref="A21:I22"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A31:O31"/>
+    <mergeCell ref="A32:O32"/>
+    <mergeCell ref="J36:O38"/>
+    <mergeCell ref="A34:O34"/>
+    <mergeCell ref="A35:O35"/>
     <mergeCell ref="A25:O25"/>
     <mergeCell ref="A26:O26"/>
-    <mergeCell ref="A27:O27"/>
-    <mergeCell ref="A28:O28"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="A30:O30"/>
-    <mergeCell ref="A31:O31"/>
-    <mergeCell ref="A32:O32"/>
+    <mergeCell ref="F38:H38"/>
     <mergeCell ref="A33:O33"/>
-    <mergeCell ref="A34:O34"/>
-    <mergeCell ref="A35:O35"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:G7"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J36:O38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -7136,261 +7033,261 @@
       <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="13"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="69"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="70"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="71"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="77"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="78"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10">
-      <c r="A10" s="83"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="85"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
     </row>
     <row r="11">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="77"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="78"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="82"/>
-      <c r="N11" s="82"/>
-      <c r="O11" s="82"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="83"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="84"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="85"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="88"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="30"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
     </row>
     <row r="13">
-      <c r="A13" s="76"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="77"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="78"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="82"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
     </row>
     <row r="14">
-      <c r="A14" s="83"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="84"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="85"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="87"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="89"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="76"/>
-      <c r="B15" s="76"/>
-      <c r="C15" s="77"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="78"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="82"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
     </row>
     <row r="16">
-      <c r="A16" s="83"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="85"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="87"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="89"/>
-      <c r="N16" s="89"/>
-      <c r="O16" s="89"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
     </row>
     <row r="17">
-      <c r="A17" s="76"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="77"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="78"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="82"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
     </row>
     <row r="18">
-      <c r="A18" s="83"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="84"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="85"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="88"/>
-      <c r="M18" s="89"/>
-      <c r="N18" s="89"/>
-      <c r="O18" s="89"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
     </row>
     <row r="19">
-      <c r="A19" s="76"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="77"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="78"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
     </row>
     <row r="20">
-      <c r="A20" s="83"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="84"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="85"/>
-      <c r="J20" s="86"/>
-      <c r="K20" s="87"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="89"/>
-      <c r="N20" s="89"/>
-      <c r="O20" s="89"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="91" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="92" t="s">
+      <c r="K21" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="93" t="s">
+      <c r="L21" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="O21" s="94" t="s">
-        <v>18</v>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="95"/>
-      <c r="K22" s="96"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="98"/>
-      <c r="O22" s="98"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="40"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="99"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -7405,89 +7302,89 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="8"/>
-      <c r="Q23" s="12" t="s">
+      <c r="Q23" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="44"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="45"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="45"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="O28" s="25"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="45"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="44"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="45"/>
+      <c r="O31" s="25"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="44"/>
+      <c r="O32" s="25"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="45"/>
+      <c r="O33" s="25"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="44"/>
+      <c r="O34" s="25"/>
+      <c r="Q34" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="46"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="15"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="51" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="100"/>
-      <c r="O24" s="29"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="101"/>
-      <c r="O25" s="29"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="100"/>
-      <c r="O26" s="29"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="101"/>
-      <c r="O27" s="29"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="100"/>
-      <c r="O28" s="29"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="101"/>
-      <c r="O29" s="29"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="100"/>
-      <c r="O30" s="29"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="101"/>
-      <c r="O31" s="29"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="100"/>
-      <c r="O32" s="29"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="101"/>
-      <c r="O33" s="29"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="100"/>
-      <c r="O34" s="29"/>
-      <c r="Q34" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="102"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="16"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="103" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="104"/>
-      <c r="C36" s="104"/>
-      <c r="D36" s="104"/>
-      <c r="E36" s="105"/>
-      <c r="F36" s="105"/>
-      <c r="G36" s="106"/>
-      <c r="H36" s="105"/>
-      <c r="I36" s="107" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="108"/>
+      <c r="J36" s="52"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -7495,48 +7392,50 @@
       <c r="O36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="109"/>
-      <c r="B37" s="105"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="105"/>
-      <c r="E37" s="105"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="106"/>
-      <c r="H37" s="105"/>
-      <c r="I37" s="107" t="s">
+      <c r="A37" s="53"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="O37" s="25"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="55"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O37" s="29"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="110" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="111"/>
-      <c r="C38" s="112" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="113"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="114"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="16"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="15"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="12"/>
+      <c r="A39" s="11"/>
     </row>
     <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="C41" s="59"/>
+    </row>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="I43" s="12"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -8496,63 +8395,65 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="58">
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="A21:I22"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A27:O27"/>
     <mergeCell ref="A25:O25"/>
     <mergeCell ref="A26:O26"/>
-    <mergeCell ref="A27:O27"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C6:G7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="A34:O34"/>
+    <mergeCell ref="A33:O33"/>
     <mergeCell ref="A28:O28"/>
     <mergeCell ref="A29:O29"/>
-    <mergeCell ref="A30:O30"/>
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="A32:O32"/>
-    <mergeCell ref="A33:O33"/>
-    <mergeCell ref="A34:O34"/>
+    <mergeCell ref="J36:O38"/>
     <mergeCell ref="A35:O35"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:G7"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="J36:O38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="F38:H38"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.7874015748031497" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.7874015748031497"/>
@@ -8575,79 +8476,124 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="26"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="30"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="26"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="63"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="50"/>
+      <c r="B8" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="115"/>
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="119"/>
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="120"/>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="117"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="121"/>
-      <c r="G5" s="29"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="119"/>
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="120"/>
-      <c r="G6" s="29"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="122"/>
-      <c r="B7" s="122"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="124"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="124"/>
+      <c r="F8" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="50"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -9630,17 +9576,19 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
+  <mergeCells count="12">
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:I2"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>